<commit_message>
Adding open extent report feature
</commit_message>
<xml_diff>
--- a/xframium-excel/resources/TestData.xlsx
+++ b/xframium-excel/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manjunathda/git/Calm/xframium-excel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D942C11D-5CB7-FE40-BA5F-99B39835F43E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D62D40-3F58-7447-97F3-EAE69E32803B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Delete</t>
+  </si>
+  <si>
+    <t>DS002</t>
   </si>
 </sst>
 </file>
@@ -519,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,9 +573,24 @@
       <c r="E2" s="2"/>
       <c r="F2" s="6"/>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F0765AC8-896B-744D-9459-713728B73CCD}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{EB5E7B8F-2873-0349-9A4F-B898A6566E49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -583,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6479F0D8-BFBF-A046-8E8B-3CA68551D7DA}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>

</xml_diff>

<commit_message>
Changed Website to Amazon and Implemented Login and Logout methods.
</commit_message>
<xml_diff>
--- a/xframium-excel/resources/TestData.xlsx
+++ b/xframium-excel/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manjunathda/git/Calm/xframium-excel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F6B73A-4D40-4E43-9D06-58C82C9CEFE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488E3B6-CEA7-AC49-990A-66F874C87484}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,7 +127,7 @@
     <t>Superispower@8</t>
   </si>
   <si>
-    <t>Hello, manjunathA</t>
+    <t>Hello, manjunath</t>
   </si>
 </sst>
 </file>

</xml_diff>